<commit_message>
fixed page 3 path, and query
</commit_message>
<xml_diff>
--- a/static/Certificate_Page3.xlsx
+++ b/static/Certificate_Page3.xlsx
@@ -525,7 +525,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="14" customWidth="1" min="9" max="9"/>
+    <col width="15" customWidth="1" min="9" max="9"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -674,7 +674,7 @@
     <row r="18">
       <c r="A18" s="7" t="inlineStr">
         <is>
-          <t>This is to certify that IMEE JANINE O. ABALON has graduated with the degree of Bachelor</t>
+          <t>This is to certify that Ms. IMEE JANINE O. ABALON has graduated with the degree of</t>
         </is>
       </c>
       <c r="B18" s="8" t="n"/>
@@ -689,7 +689,7 @@
     <row r="19">
       <c r="A19" s="9" t="inlineStr">
         <is>
-          <t>in Science in Industrial Education (BSIE), major in Food and Service Management from Bicol</t>
+          <t>Bachelor of Science in Industrial Education (BSIE), major in Food and Service Management</t>
         </is>
       </c>
       <c r="B19" s="8" t="n"/>
@@ -704,7 +704,7 @@
     <row r="20">
       <c r="A20" s="9" t="inlineStr">
         <is>
-          <t>Univeristy College of Industrial Technology, East Campus, Legazpi City on March 28, 2015 per</t>
+          <t>from College Of Industrial Technology, East Campus, Legazpi City, Albay on March 28, 2015</t>
         </is>
       </c>
       <c r="B20" s="8" t="n"/>
@@ -719,7 +719,7 @@
     <row r="21">
       <c r="A21" s="9" t="inlineStr">
         <is>
-          <t>Board of Regents Referendum No. 02-A, s. 2015 having a General Weighted Average (GWA)</t>
+          <t>per Board of Regents Referendum No. 02-A, s. 2015 having a General Weighted Average (GWA)</t>
         </is>
       </c>
       <c r="B21" s="8" t="n"/>
@@ -760,7 +760,7 @@
     <row r="24">
       <c r="A24" s="7" t="inlineStr">
         <is>
-          <t>Issued this 28th day of February, 2017 upon the request of interested party for reference</t>
+          <t>Issued this 15th day of July, 2021 upon the request of interested party for reference purposes.</t>
         </is>
       </c>
       <c r="B24" s="8" t="n"/>
@@ -773,11 +773,7 @@
       <c r="I24" s="8" t="n"/>
     </row>
     <row r="25">
-      <c r="A25" s="9" t="inlineStr">
-        <is>
-          <t>purposes.</t>
-        </is>
-      </c>
+      <c r="A25" s="8" t="n"/>
       <c r="B25" s="8" t="n"/>
       <c r="C25" s="8" t="n"/>
       <c r="D25" s="8" t="n"/>
@@ -790,7 +786,7 @@
     <row r="30">
       <c r="G30" s="10" t="inlineStr">
         <is>
-          <t>SOPHIA A. ROMERO</t>
+          <t>CORAZON N. BAZAR</t>
         </is>
       </c>
     </row>
@@ -821,7 +817,7 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="22">
+  <mergeCells count="21">
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A2:I2"/>
     <mergeCell ref="A3:I3"/>
@@ -838,7 +834,6 @@
     <mergeCell ref="A21:I21"/>
     <mergeCell ref="A22:I22"/>
     <mergeCell ref="A24:I24"/>
-    <mergeCell ref="A25:I25"/>
     <mergeCell ref="G30:I30"/>
     <mergeCell ref="G31:I31"/>
     <mergeCell ref="A40:B40"/>

</xml_diff>